<commit_message>
End of the semester push
</commit_message>
<xml_diff>
--- a/TA SCHEDULE.xlsx
+++ b/TA SCHEDULE.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfdeblasio/My Drive (danfdeblasio@gmail.com)/Classes/CS2101.2202/CS2101.CS2202.Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE429F48-A18D-824C-B437-F8A49E2580B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458AE44C-025C-3C43-BBFF-2CAB27029B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18060" yWindow="1660" windowWidth="34460" windowHeight="26460" xr2:uid="{83CA6D1F-4B7B-D74B-9C4E-C1B71C23FF27}"/>
+    <workbookView xWindow="12940" yWindow="760" windowWidth="34460" windowHeight="26460" activeTab="1" xr2:uid="{83CA6D1F-4B7B-D74B-9C4E-C1B71C23FF27}"/>
   </bookViews>
   <sheets>
-    <sheet name="Spring23" sheetId="2" r:id="rId1"/>
+    <sheet name="Spring23-v1" sheetId="2" r:id="rId1"/>
+    <sheet name="Spring23-v2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
   <si>
     <t>Monday</t>
   </si>
@@ -83,6 +84,15 @@
   <si>
     <t>Montoya Sanchez
 4:00-6:00</t>
+  </si>
+  <si>
+    <t>Montoya Sanchez
+(virtual only)
+2:00-4:00</t>
+  </si>
+  <si>
+    <t>DeBlasio
+10:00-11:00</t>
   </si>
 </sst>
 </file>
@@ -196,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -210,55 +220,54 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,19 +583,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B75F5B-F6D5-F04B-AA0C-AA746A42E9FC}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="4.83203125" style="2" customWidth="1"/>
     <col min="3" max="7" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="101" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" ht="34" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
       <c r="C1" s="8" t="s">
         <v>0</v>
@@ -616,15 +629,15 @@
       <c r="B2" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -636,11 +649,11 @@
     </row>
     <row r="3" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="9"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -652,11 +665,11 @@
     </row>
     <row r="4" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -668,11 +681,11 @@
     </row>
     <row r="5" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="13"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="10"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -686,15 +699,15 @@
       <c r="B6" s="7">
         <v>0.375</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -706,11 +719,11 @@
     </row>
     <row r="7" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="9"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -722,11 +735,11 @@
     </row>
     <row r="8" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="5"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="12"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -738,11 +751,11 @@
     </row>
     <row r="9" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="13"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="10"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -756,11 +769,11 @@
       <c r="B10" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="9"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -772,11 +785,11 @@
     </row>
     <row r="11" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="9"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -788,15 +801,15 @@
     </row>
     <row r="12" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="21" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="21" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="12"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -808,11 +821,11 @@
     </row>
     <row r="13" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="13"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="10"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -826,11 +839,11 @@
       <c r="B14" s="4">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="9"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -842,11 +855,11 @@
     </row>
     <row r="15" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="9"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -858,11 +871,11 @@
     </row>
     <row r="16" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="12"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -874,11 +887,11 @@
     </row>
     <row r="17" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="10"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -892,15 +905,15 @@
       <c r="B18" s="7">
         <v>0.5</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="10" t="s">
+      <c r="E18" s="11"/>
+      <c r="F18" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="15"/>
+      <c r="G18" s="11"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -912,11 +925,11 @@
     </row>
     <row r="19" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="5"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="16"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="12"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -928,11 +941,11 @@
     </row>
     <row r="20" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="16"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="12"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -944,11 +957,11 @@
     </row>
     <row r="21" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="17"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="13"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -962,13 +975,13 @@
       <c r="B22" s="4">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="22" t="s">
+      <c r="C22" s="2"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="9"/>
+      <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -980,11 +993,11 @@
     </row>
     <row r="23" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="9"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -996,15 +1009,15 @@
     </row>
     <row r="24" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="5"/>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="25" t="s">
+      <c r="D24" s="9"/>
+      <c r="E24" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="12"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="9"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1016,11 +1029,11 @@
     </row>
     <row r="25" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="10"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -1034,11 +1047,11 @@
       <c r="B26" s="4">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="16"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="12"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -1050,11 +1063,11 @@
     </row>
     <row r="27" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="5"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="16"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="12"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -1066,11 +1079,11 @@
     </row>
     <row r="28" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="5"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="16"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="12"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -1082,11 +1095,11 @@
     </row>
     <row r="29" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="17"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="13"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -1100,13 +1113,13 @@
       <c r="B30" s="7">
         <v>0.625</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="18"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="14"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -1118,11 +1131,11 @@
     </row>
     <row r="31" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="5"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="16"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="12"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -1134,11 +1147,11 @@
     </row>
     <row r="32" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="5"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="16"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="12"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -1150,11 +1163,11 @@
     </row>
     <row r="33" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="17"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="13"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -1168,13 +1181,13 @@
       <c r="B34" s="7">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="26" t="s">
+      <c r="C34" s="18"/>
+      <c r="D34" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="18"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="14"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -1186,11 +1199,11 @@
     </row>
     <row r="35" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="5"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="16"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="12"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
@@ -1202,11 +1215,11 @@
     </row>
     <row r="36" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="5"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
@@ -1218,11 +1231,11 @@
     </row>
     <row r="37" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -1236,11 +1249,11 @@
       <c r="B38" s="7">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -1252,11 +1265,11 @@
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B39" s="3"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
@@ -1268,7 +1281,7 @@
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C40" s="2"/>
-      <c r="D40" s="25"/>
+      <c r="D40" s="15"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -1284,7 +1297,7 @@
     <row r="41" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="25"/>
+      <c r="D41" s="15"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -1301,11 +1314,11 @@
       <c r="B42" s="7">
         <v>0.75</v>
       </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -1524,20 +1537,996 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F22:F29"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="D6:D11"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="F6:F11"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="F18:F21"/>
     <mergeCell ref="C24:C27"/>
     <mergeCell ref="E24:E27"/>
     <mergeCell ref="D34:D41"/>
     <mergeCell ref="C30:C37"/>
     <mergeCell ref="D18:D21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="44" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11B50432-7715-A94B-8CD3-5BEEE68C6D03}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L51" sqref="L51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.83203125" style="2" customWidth="1"/>
+    <col min="3" max="7" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" ht="34" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="1"/>
+      <c r="C1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="5"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="5"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="6"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="5"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="5"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="6"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="7">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="23"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="5"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="5"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="6"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="5"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="5"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="6"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="5"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="5"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+    </row>
+    <row r="21" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="6"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+    </row>
+    <row r="22" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="5"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+    </row>
+    <row r="24" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="5"/>
+      <c r="C24" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+    </row>
+    <row r="25" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="6"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+    </row>
+    <row r="26" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="4">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+    </row>
+    <row r="27" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="5"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="5"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="6"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+    </row>
+    <row r="30" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="7">
+        <v>0.625</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+    </row>
+    <row r="31" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="5"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+    </row>
+    <row r="32" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="5"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+    </row>
+    <row r="33" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="6"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+    </row>
+    <row r="34" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="7">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C34" s="18"/>
+      <c r="D34" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+    </row>
+    <row r="35" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="5"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+    </row>
+    <row r="36" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="5"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+    </row>
+    <row r="37" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="6"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+    </row>
+    <row r="38" spans="2:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="7">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C38" s="11"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B39" s="3"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C40" s="2"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B42" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="G26:G33"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="F22:F29"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="C30:C37"/>
+    <mergeCell ref="D34:D41"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="F2:F5"/>
     <mergeCell ref="D6:D11"/>
-    <mergeCell ref="D12:D15"/>
     <mergeCell ref="F6:F11"/>
     <mergeCell ref="F12:F15"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="F22:F29"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="E10:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="44" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>